<commit_message>
added excel functions on offer/request files
</commit_message>
<xml_diff>
--- a/Demandes_2022.xlsx
+++ b/Demandes_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayeu\CASSIOPEE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaume12321/Documents/GitHub/carpooling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8EF3DA-58EA-49EF-A3C6-ED00116A241D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A86A45-4170-3840-ACFC-C4B07134FF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8620" yWindow="4780" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demandes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="79">
   <si>
     <t>Prénom</t>
   </si>
@@ -258,6 +258,18 @@
   </si>
   <si>
     <t>Pair</t>
+  </si>
+  <si>
+    <t>Nombre de Oui</t>
+  </si>
+  <si>
+    <t>Nombre de Pair</t>
+  </si>
+  <si>
+    <t>Nombre de Impair</t>
+  </si>
+  <si>
+    <t>Nombre de Oui, Impair, Pair sur une semaine</t>
   </si>
 </sst>
 </file>
@@ -353,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,6 +382,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,20 +691,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE22" sqref="AE22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
     <col min="28" max="28" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -776,7 +790,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -862,7 +876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -948,7 +962,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1048,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1120,7 +1134,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1292,7 +1306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -1378,7 +1392,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1464,7 +1478,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1550,7 +1564,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -1636,7 +1650,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1722,7 +1736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1808,7 +1822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1894,7 +1908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
@@ -1980,7 +1994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -2066,7 +2080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2152,7 +2166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -2324,7 +2338,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -2410,7 +2424,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
@@ -2496,7 +2510,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2582,7 +2596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -2668,7 +2682,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -2754,7 +2768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -2840,7 +2854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -2926,7 +2940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -3012,7 +3026,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -3098,7 +3112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -3184,7 +3198,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -3270,7 +3284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
@@ -3356,7 +3370,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>72</v>
       </c>
@@ -3442,7 +3456,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -3528,7 +3542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
@@ -3614,7 +3628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -3700,7 +3714,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -3786,7 +3800,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>63</v>
       </c>
@@ -3872,7 +3886,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>64</v>
       </c>
@@ -3958,7 +3972,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
@@ -4044,7 +4058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -4130,7 +4144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
@@ -4216,7 +4230,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>67</v>
       </c>
@@ -4302,7 +4316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>68</v>
       </c>
@@ -4388,7 +4402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>69</v>
       </c>
@@ -4472,6 +4486,42 @@
       </c>
       <c r="AB44" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47">
+        <f>COUNTIF(B2:AB44, "Oui")</f>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <f>COUNTIF(B3:AB45, "Pair")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="8">
+        <f>COUNTIF(B2:AB44, "Impair")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50">
+        <f>SUM(B47:B49)</f>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -4491,6 +4541,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76424c09-1f09-411f-a39d-769041d462c4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7a404e10-278a-4ba0-976a-2af2db24d8c8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D879E14ABC0C0949BB8A7AD4556264B4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="29e167d0c93a63a8286ab5675afb04b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="76424c09-1f09-411f-a39d-769041d462c4" xmlns:ns3="7a404e10-278a-4ba0-976a-2af2db24d8c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24b04f44be219caa97f08e98b44d806e" ns2:_="" ns3:_="">
     <xsd:import namespace="76424c09-1f09-411f-a39d-769041d462c4"/>
@@ -4691,17 +4752,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76424c09-1f09-411f-a39d-769041d462c4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7a404e10-278a-4ba0-976a-2af2db24d8c8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4E4CB1-F1F2-4CFA-B19C-822160ACCD03}">
   <ds:schemaRefs>
@@ -4711,6 +4761,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{679BA0CA-EA92-41F7-9872-0C887B76F540}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76424c09-1f09-411f-a39d-769041d462c4"/>
+    <ds:schemaRef ds:uri="7a404e10-278a-4ba0-976a-2af2db24d8c8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9D01E8-DBD3-48A6-B171-42327A7D97A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4727,15 +4788,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{679BA0CA-EA92-41F7-9872-0C887B76F540}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76424c09-1f09-411f-a39d-769041d462c4"/>
-    <ds:schemaRef ds:uri="7a404e10-278a-4ba0-976a-2af2db24d8c8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
work on other data
</commit_message>
<xml_diff>
--- a/Demandes_2022.xlsx
+++ b/Demandes_2022.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaume12321/Documents/GitHub/carpooling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDF0C45-A302-0747-9017-C4BC48A38379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D9A94A-148E-C845-B670-AEFAE653BE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14600" yWindow="500" windowWidth="14200" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Demandes" sheetId="1" r:id="rId1"/>
+    <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -4362,17 +4362,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76424c09-1f09-411f-a39d-769041d462c4">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7a404e10-278a-4ba0-976a-2af2db24d8c8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D879E14ABC0C0949BB8A7AD4556264B4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="29e167d0c93a63a8286ab5675afb04b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="76424c09-1f09-411f-a39d-769041d462c4" xmlns:ns3="7a404e10-278a-4ba0-976a-2af2db24d8c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24b04f44be219caa97f08e98b44d806e" ns2:_="" ns3:_="">
     <xsd:import namespace="76424c09-1f09-411f-a39d-769041d462c4"/>
@@ -4573,6 +4562,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76424c09-1f09-411f-a39d-769041d462c4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7a404e10-278a-4ba0-976a-2af2db24d8c8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4583,17 +4583,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{679BA0CA-EA92-41F7-9872-0C887B76F540}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76424c09-1f09-411f-a39d-769041d462c4"/>
-    <ds:schemaRef ds:uri="7a404e10-278a-4ba0-976a-2af2db24d8c8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9D01E8-DBD3-48A6-B171-42327A7D97A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4612,6 +4601,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{679BA0CA-EA92-41F7-9872-0C887B76F540}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76424c09-1f09-411f-a39d-769041d462c4"/>
+    <ds:schemaRef ds:uri="7a404e10-278a-4ba0-976a-2af2db24d8c8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA4E4CB1-F1F2-4CFA-B19C-822160ACCD03}">
   <ds:schemaRefs>

</xml_diff>